<commit_message>
Solved training problems, ready to roll
</commit_message>
<xml_diff>
--- a/results/test_results.xlsx
+++ b/results/test_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,541 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.08940200973474279</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.089</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.08914324120462173</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.1002626970827905</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1001132428109867</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>10</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.099837209266712</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.09989697841238747</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.1014656517005107</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.1016042081820729</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.1017087243261681</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.101</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.1012854989517913</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.1116839403410627</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.111</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.1112856728672684</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9.700000000000001</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.09718331607848341</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.097</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.09703348226279994</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.1129268993858945</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.112</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.1123392805369265</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.09778284629050643</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.09777859833973764</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.1139300491955115</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.114</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.1139293818086055</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.09511519919779822</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.09503644558275942</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.1114568465404394</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.111</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.1112063287118179</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>50.82742316784869</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.508274231678487</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.508274231678487</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.508274231678487</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>51.91489361702127</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.519249560397596</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.5191489361702127</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.519198208557437</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>51.01654846335697</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.5100972430478454</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.5101654846335697</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.5101309099656703</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>49.88179669030733</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.4987481027651594</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.4988179669030733</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.4987825912776163</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>52.95508274231678</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.4896169755726166</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.5295508274231678</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.409951480439783</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>50.49645390070921</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.5049300468157141</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.5049645390070922</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.5049471806212312</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>49.69267139479906</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.4968565793847117</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.4969267139479905</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.4968912048296075</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>51.58392434988179</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.5157718131891885</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.5158392434988179</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.5158050693096974</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>51.15839243498817</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.5115498993837456</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.5115839243498818</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.5115667980723322</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>50.02513826043238</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.5075075075075075</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.5024777006937562</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.5049800796812749</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>49.37154348919055</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0.5009487666034156</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.5232903865213082</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.5118759088705769</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>49.42182001005531</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.004955401387512388</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.00984251968503937</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>50.82956259426847</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.5091337654684738</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.8562933597621407</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.6385809312638581</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>48.46656611362494</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0.4916142557651992</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.464816650148662</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.4778400407539481</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>48.01407742584213</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.4881291547958215</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.5094152626362736</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.498545101842871</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>QCONV_011</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1.563153346882591</v>
+      </c>
+      <c r="B32" t="n">
+        <v>99.38775510204081</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.9938796079950354</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.9938775510204082</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.9938775446455067</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>test_model</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>